<commit_message>
Linear feet + Category Space + Count of adaptation to FABRICARE changes
</commit_message>
<xml_diff>
--- a/Projects/PNGAMERICA/Data/Template_v4.2.xlsx
+++ b/Projects/PNGAMERICA/Data/Template_v4.2.xlsx
@@ -25,32 +25,33 @@
     <sheet name="average shelf" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3749" uniqueCount="205">
   <si>
     <t>kpi Name</t>
   </si>
@@ -1052,12 +1053,12 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="C419 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="91.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="91.8016194331984"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -1149,15 +1150,15 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="C419 C6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="166.890688259109"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="168.392712550607"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1308,17 +1309,17 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="1" sqref="C419 E28"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.9473684210526"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1404,18 +1405,18 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="C419 B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.4534412955466"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.2753036437247"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1581,14 +1582,14 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C419 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="113.331983805668"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.1983805668016"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="114.295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.7004048582996"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
@@ -1652,15 +1653,15 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="1" sqref="C419 F18"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.663967611336"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.1983805668016"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1836,12 +1837,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="C419 A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1896,15 +1897,15 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="C419 B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="119.546558704453"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.3036437246964"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="120.615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.7732793522267"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2322,15 +2323,15 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="1" sqref="C419 B32"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="119.651821862348"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.3076923076923"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="120.724696356275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.9473684210526"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="62.1295546558704"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3285,16 +3286,16 @@
   <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="1" sqref="C419 A81"/>
+      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.546558704453"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.51012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4394,17 +4395,17 @@
   <dimension ref="A1:K78"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A75" activeCellId="1" sqref="C419 A75"/>
+      <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="169.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="171.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5753,14 +5754,14 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="C419 B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="91.6923076923077"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="92.4453441295547"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2753036437247"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6031,14 +6032,14 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="1" sqref="C419 D33"/>
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="113.331983805668"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.1983805668016"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="114.295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.7004048582996"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6764,15 +6765,15 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="1" sqref="C419 B23"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="132.825910931174"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.919028340081"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="134.004048582996"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3441295546559"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7150,18 +7151,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F455"/>
+  <dimension ref="A1:F427"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A389" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C419" activeCellId="0" sqref="C419"/>
+      <selection pane="topLeft" activeCell="C413" activeCellId="0" sqref="C413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="113.331983805668"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="95.0161943319838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="114.295546558704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="95.8704453441296"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -14407,83 +14408,36 @@
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C441" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C442" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C443" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C444" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C445" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C446" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C447" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C448" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C449" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C450" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C451" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C452" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C453" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C454" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C455" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
+    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:F357"/>
+  <autoFilter ref="A1:F337"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>